<commit_message>
Translation of the excel sheets
</commit_message>
<xml_diff>
--- a/koboforms/Budgets.xlsx
+++ b/koboforms/Budgets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deo/anticipatoryactiondecisions/koboforms/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dasdoresngueussiengamini/working/AA_projets/general/aadecisionoverviewFR/koboforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1063C8D2-C1AE-7B48-B723-8FA0CFD86238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32557BFB-F022-AF4B-8FC4-9A59E9C14567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="1780" windowWidth="28040" windowHeight="17440" xr2:uid="{05574417-E28B-7A44-8D51-6FA488FA6DA5}"/>
+    <workbookView xWindow="2200" yWindow="1000" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{05574417-E28B-7A44-8D51-6FA488FA6DA5}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>type</t>
   </si>
@@ -63,77 +63,80 @@
     <t>version</t>
   </si>
   <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>q1</t>
+  </si>
+  <si>
+    <t>q2</t>
+  </si>
+  <si>
+    <t>list_name</t>
+  </si>
+  <si>
+    <t>yes_no</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>q3</t>
+  </si>
+  <si>
+    <t>q4</t>
+  </si>
+  <si>
+    <t>appearance</t>
+  </si>
+  <si>
+    <t>q0</t>
+  </si>
+  <si>
+    <t>select_one yes_no</t>
+  </si>
+  <si>
+    <t>Votre adresse e‑mail</t>
+  </si>
+  <si>
+    <t>De combien de millions l’acteur aurait‑il besoin sur les cinq années ?</t>
+  </si>
+  <si>
+    <t>Quel taux d’actions le bailleur peut‑il financer ?</t>
+  </si>
+  <si>
+    <t>Le bailleur peut‑il financer le taux d’actions que l’acteur souhaite entreprendre ?</t>
+  </si>
+  <si>
+    <t>Le bailleur et l’acteur devraient négocier le taux d’action qui pourrait être appliqué. Quel taux est convenu (y a‑t‑il un accord) ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les contraintes budgétaires ont‑elles un impact sur les fréquences d’action ? </t>
+  </si>
+  <si>
+    <t>Oui</t>
+  </si>
+  <si>
+    <t>Non</t>
+  </si>
+  <si>
+    <t>Budgets FR</t>
+  </si>
+  <si>
+    <t>BudgetsFR</t>
+  </si>
+  <si>
     <t>v1</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>q1</t>
-  </si>
-  <si>
-    <t>q2</t>
-  </si>
-  <si>
-    <t>Your email</t>
-  </si>
-  <si>
-    <t>list_name</t>
-  </si>
-  <si>
-    <t>yes_no</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>q3</t>
-  </si>
-  <si>
-    <t>q4</t>
-  </si>
-  <si>
-    <t>appearance</t>
-  </si>
-  <si>
-    <t>q0</t>
-  </si>
-  <si>
-    <t>select_one yes_no</t>
-  </si>
-  <si>
-    <t>Budgets</t>
-  </si>
-  <si>
-    <t>How many millions would the actor need over the 5 years?</t>
-  </si>
-  <si>
-    <t>What rate of actions can the funder fund?</t>
-  </si>
-  <si>
-    <t>Can the funder fund the rate of actions that the actor wants to take?</t>
-  </si>
-  <si>
-    <t>The Funder and the Actor should negotiate what the rate of action that could occur. What rate is agreed upon (is anything agreed upon)?</t>
-  </si>
-  <si>
-    <t>Do budget constraints impact action frequencies?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -161,6 +164,12 @@
       <color rgb="FF1F1F1F"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -513,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{994C7F9E-9867-6243-AAB9-77628DC2993D}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -533,10 +542,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -544,10 +553,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>4</v>
@@ -558,10 +567,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -572,10 +581,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>
@@ -583,13 +592,13 @@
     </row>
     <row r="5" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
@@ -600,24 +609,24 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
@@ -633,14 +642,14 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -651,24 +660,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -678,15 +687,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8DF2FC2-2B0D-0B42-899E-2C094C966549}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -696,19 +705,21 @@
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Kobo forms in French
</commit_message>
<xml_diff>
--- a/koboforms/Budgets.xlsx
+++ b/koboforms/Budgets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dasdoresngueussiengamini/working/AA_projets/general/aadecisionoverviewFR/koboforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32557BFB-F022-AF4B-8FC4-9A59E9C14567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E9900F6-3919-9B45-A217-13427FD44CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="1000" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{05574417-E28B-7A44-8D51-6FA488FA6DA5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>type</t>
   </si>
@@ -123,13 +123,10 @@
     <t>Non</t>
   </si>
   <si>
-    <t>Budgets FR</t>
-  </si>
-  <si>
-    <t>BudgetsFR</t>
-  </si>
-  <si>
     <t>v1</t>
+  </si>
+  <si>
+    <t>Budgets</t>
   </si>
 </sst>
 </file>
@@ -690,7 +687,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -709,13 +706,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
         <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>